<commit_message>
Updated the PCB: made it smaller, compact routing, thicker traces, better readable silk screen markings. Rectified eroneous comment.
</commit_message>
<xml_diff>
--- a/schematics/pico-glitcher-v1.1-BOM.xlsx
+++ b/schematics/pico-glitcher-v1.1-BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
   <si>
     <t>Comment</t>
   </si>
@@ -64,10 +64,10 @@
     <t>C8</t>
   </si>
   <si>
-    <t>SMD,D5xL5.8mm</t>
-  </si>
-  <si>
-    <t>C336199</t>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>C178580</t>
   </si>
   <si>
     <t>10kΩ</t>
@@ -115,10 +115,10 @@
     <t>R12, R13, R14, R15</t>
   </si>
   <si>
-    <t>1206</t>
-  </si>
-  <si>
-    <t>C840645</t>
+    <t>0603x4</t>
+  </si>
+  <si>
+    <t>C396839</t>
   </si>
   <si>
     <t>4x 100Ω 1206 Resistor Array</t>
@@ -127,7 +127,7 @@
     <t>R16, R17, R18, R19</t>
   </si>
   <si>
-    <t>C5568274</t>
+    <t>C396838</t>
   </si>
   <si>
     <t>IRLML2502</t>
@@ -226,9 +226,6 @@
     <t>S1</t>
   </si>
   <si>
-    <t>SMD</t>
-  </si>
-  <si>
     <t>C160878</t>
   </si>
   <si>
@@ -289,7 +286,7 @@
     <t>S_RST</t>
   </si>
   <si>
-    <t>C483806</t>
+    <t>C2845324</t>
   </si>
 </sst>
 </file>
@@ -1779,100 +1776,100 @@
         <v>70</v>
       </c>
       <c r="C20" t="s" s="4">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s" s="4">
         <v>71</v>
-      </c>
-      <c r="D20" t="s" s="4">
-        <v>72</v>
       </c>
       <c r="E20" s="6"/>
     </row>
     <row r="21" ht="14.7" customHeight="1">
       <c r="A21" t="s" s="6">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s" s="5">
         <v>73</v>
       </c>
-      <c r="B21" t="s" s="5">
+      <c r="C21" t="s" s="4">
         <v>74</v>
       </c>
-      <c r="C21" t="s" s="4">
+      <c r="D21" t="s" s="4">
         <v>75</v>
-      </c>
-      <c r="D21" t="s" s="4">
-        <v>76</v>
       </c>
       <c r="E21" s="6"/>
     </row>
     <row r="22" ht="50.65" customHeight="1">
       <c r="A22" t="s" s="4">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s" s="5">
         <v>77</v>
       </c>
-      <c r="B22" t="s" s="5">
+      <c r="C22" t="s" s="4">
         <v>78</v>
       </c>
-      <c r="C22" t="s" s="4">
+      <c r="D22" t="s" s="4">
         <v>79</v>
-      </c>
-      <c r="D22" t="s" s="4">
-        <v>80</v>
       </c>
       <c r="E22" s="6"/>
     </row>
     <row r="23" ht="14.7" customHeight="1">
       <c r="A23" t="s" s="4">
+        <v>80</v>
+      </c>
+      <c r="B23" t="s" s="5">
         <v>81</v>
       </c>
-      <c r="B23" t="s" s="5">
+      <c r="C23" t="s" s="4">
+        <v>78</v>
+      </c>
+      <c r="D23" t="s" s="4">
         <v>82</v>
-      </c>
-      <c r="C23" t="s" s="4">
-        <v>79</v>
-      </c>
-      <c r="D23" t="s" s="4">
-        <v>83</v>
       </c>
       <c r="E23" s="6"/>
     </row>
     <row r="24" ht="38.65" customHeight="1">
       <c r="A24" t="s" s="4">
+        <v>83</v>
+      </c>
+      <c r="B24" t="s" s="5">
         <v>84</v>
       </c>
-      <c r="B24" t="s" s="5">
+      <c r="C24" t="s" s="4">
+        <v>78</v>
+      </c>
+      <c r="D24" t="s" s="6">
         <v>85</v>
-      </c>
-      <c r="C24" t="s" s="4">
-        <v>79</v>
-      </c>
-      <c r="D24" t="s" s="6">
-        <v>86</v>
       </c>
       <c r="E24" s="6"/>
     </row>
     <row r="25" ht="14.7" customHeight="1">
       <c r="A25" t="s" s="4">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s" s="5">
         <v>87</v>
       </c>
-      <c r="B25" t="s" s="5">
+      <c r="C25" t="s" s="6">
+        <v>78</v>
+      </c>
+      <c r="D25" t="s" s="4">
         <v>88</v>
-      </c>
-      <c r="C25" t="s" s="6">
-        <v>79</v>
-      </c>
-      <c r="D25" t="s" s="4">
-        <v>89</v>
       </c>
       <c r="E25" s="6"/>
     </row>
     <row r="26" ht="14.7" customHeight="1">
       <c r="A26" t="s" s="6">
+        <v>89</v>
+      </c>
+      <c r="B26" t="s" s="5">
         <v>90</v>
       </c>
-      <c r="B26" t="s" s="5">
+      <c r="C26" t="s" s="4">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s" s="4">
         <v>91</v>
-      </c>
-      <c r="C26" t="s" s="4">
-        <v>71</v>
-      </c>
-      <c r="D26" t="s" s="4">
-        <v>92</v>
       </c>
       <c r="E26" s="6"/>
     </row>

</xml_diff>

<commit_message>
New feature: Genetic Algorithm that helps to find optimal parameter sets in a multidimensional parameter space
</commit_message>
<xml_diff>
--- a/schematics/pico-glitcher-v1.1-BOM.xlsx
+++ b/schematics/pico-glitcher-v1.1-BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="96">
   <si>
     <t>Comment</t>
   </si>
@@ -287,6 +287,18 @@
   </si>
   <si>
     <t>C2845324</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Pico</t>
+  </si>
+  <si>
+    <t>PICO</t>
+  </si>
+  <si>
+    <t>RPI_PICO</t>
+  </si>
+  <si>
+    <t>C7203002</t>
   </si>
 </sst>
 </file>
@@ -1469,7 +1481,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1873,6 +1885,21 @@
       </c>
       <c r="E26" s="6"/>
     </row>
+    <row r="27" ht="14.7" customHeight="1">
+      <c r="A27" t="s" s="4">
+        <v>92</v>
+      </c>
+      <c r="B27" t="s" s="5">
+        <v>93</v>
+      </c>
+      <c r="C27" t="s" s="4">
+        <v>94</v>
+      </c>
+      <c r="D27" t="s" s="4">
+        <v>95</v>
+      </c>
+      <c r="E27" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>